<commit_message>
Site updated: 2021-06-10 15:12:08
</commit_message>
<xml_diff>
--- a/DIY/download/【学科丨数学】02.xlsx
+++ b/DIY/download/【学科丨数学】02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\博客\Blog\themes\next\source\DIY\download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1A44E8-3FAE-4801-A654-6E3FA2A71ABC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4681AEC9-3F6E-4A87-9DF4-0FD1A65918FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="795" windowWidth="23325" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5925" yWindow="2190" windowWidth="20055" windowHeight="12690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,129 +25,121 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
-  <si>
-    <t>数学分析</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>线性代数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>解析几何</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>概率论与数理统计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>实分析</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>抽象代数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>初等数论</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>集合论</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数理逻辑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>泛函分析</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>范畴论</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ODE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PDE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>调和分析</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>交换代数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表示论</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>同调代数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>黎曼几何</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>复几何</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>辛几何</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>古典微分几何</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>微分拓扑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>代数拓扑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>微分流形（包括张量分析）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>高等概率论（实变之后）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点集拓扑（实变之后）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>阶段一</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>阶段二</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>阶段三</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>阶段四</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>复分析（包括多复变）</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>Analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linear Algebra</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Analytic Geometry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Probability and Statistic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complex Analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Functional Analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Real Analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Partial Differential Equation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Odinary Differential Equation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Abstract Algebra</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set Theory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elementray Number Theory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mathematical Logic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Representaion Theory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Categorical Theory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Point Set Topology</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Differnetial Manifold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commutative Algebra</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Homological Algebra</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Harmonic Analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Advanced Probability</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Riemannian Geometry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Algebraic Geometry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Algebraic Topology</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Classsical Differential Geometry</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -236,7 +228,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor rgb="FF002060"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -254,12 +246,10 @@
       <right style="dashed">
         <color theme="0" tint="-0.24994659260841701"/>
       </right>
-      <top style="dashed">
+      <top style="thin">
         <color theme="0" tint="-0.24994659260841701"/>
       </top>
-      <bottom style="dashed">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -269,12 +259,10 @@
       <right style="dashed">
         <color theme="0" tint="-0.24994659260841701"/>
       </right>
-      <top style="dashed">
+      <top style="thin">
         <color theme="0" tint="-0.24994659260841701"/>
       </top>
-      <bottom style="dashed">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -282,12 +270,10 @@
         <color theme="0" tint="-0.24994659260841701"/>
       </left>
       <right/>
-      <top style="dashed">
+      <top style="thin">
         <color theme="0" tint="-0.24994659260841701"/>
       </top>
-      <bottom style="dashed">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -295,12 +281,8 @@
       <right style="dashed">
         <color theme="0" tint="-0.24994659260841701"/>
       </right>
-      <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="dashed">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -310,12 +292,8 @@
       <right style="dashed">
         <color theme="0" tint="-0.24994659260841701"/>
       </right>
-      <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="dashed">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -323,12 +301,8 @@
         <color theme="0" tint="-0.24994659260841701"/>
       </left>
       <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="dashed">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -340,58 +314,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -674,16 +650,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:E15"/>
+  <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.25" customWidth="1"/>
-    <col min="2" max="5" width="24.75" customWidth="1"/>
+    <col min="2" max="2" width="24.75" customWidth="1"/>
+    <col min="3" max="3" width="27.125" customWidth="1"/>
+    <col min="4" max="5" width="24.75" customWidth="1"/>
     <col min="7" max="7" width="17.25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.5" bestFit="1" customWidth="1"/>
@@ -691,150 +669,140 @@
   <sheetData>
     <row r="1" spans="2:5" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:5" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="2:5" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="2:5" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="2:5" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="9"/>
+      <c r="C7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="2:5" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="18" t="s">
+    </row>
+    <row r="12" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="8"/>
-      <c r="C4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="5" spans="2:5" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="8"/>
-      <c r="C5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="6" spans="2:5" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="2:5" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="2"/>
-      <c r="C7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="2:5" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="11"/>
-      <c r="C11" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="11"/>
-      <c r="C12" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="13" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="11"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13" t="s">
-        <v>21</v>
-      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
     </row>
     <row r="14" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="11"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="15" t="s">
+      <c r="B14" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16" t="s">
+      <c r="C14" s="16"/>
+      <c r="D14" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="17"/>
+      <c r="E14" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>